<commit_message>
store CRUD structure, postman collection, updates data base
</commit_message>
<xml_diff>
--- a/Last-Bite-Backend/docs/Database.xlsx
+++ b/Last-Bite-Backend/docs/Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidsantiago/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidsantiago/Desktop/BackendMoviles/MOBILE_APP_DEV_BACKEND-S4-G4/Last-Bite-Backend/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A47D339B-FF05-F242-9016-32E0E01C0022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DE2ED2-0777-DE45-B36F-A65993028AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1480" windowWidth="23260" windowHeight="12460" firstSheet="4" activeTab="12" xr2:uid="{47F1251A-4F32-B949-8330-818A2A4EE1EB}"/>
+    <workbookView xWindow="0" yWindow="1480" windowWidth="23260" windowHeight="12460" xr2:uid="{47F1251A-4F32-B949-8330-818A2A4EE1EB}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="192">
   <si>
     <t>dstapias</t>
   </si>
@@ -616,6 +616,12 @@
   </si>
   <si>
     <t>This table stores all the products in the different cars. This products should not be deleted if the car is BILLED or PAYMENT_PROGRESS</t>
+  </si>
+  <si>
+    <t>VERIFICATION_CODE</t>
+  </si>
+  <si>
+    <t>4 digit verification code</t>
   </si>
 </sst>
 </file>
@@ -771,7 +777,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -806,22 +812,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -832,12 +823,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -852,11 +837,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1194,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E74DDD3-3953-4686-BE4A-5A727D22B079}">
   <dimension ref="A2:I61"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1212,8 +1210,8 @@
     <col min="10" max="10" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1229,17 +1227,20 @@
         <v>33</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="22"/>
       <c r="B3" s="2" t="s">
         <v>25</v>
       </c>
@@ -1253,17 +1254,20 @@
         <v>34</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
+      <c r="I3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="22"/>
       <c r="B4" s="3">
         <v>1</v>
       </c>
@@ -1277,17 +1281,20 @@
         <v>1655454544</v>
       </c>
       <c r="F4" s="3">
+        <v>1234</v>
+      </c>
+      <c r="G4" s="3">
         <v>1</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="22"/>
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -1300,18 +1307,21 @@
       <c r="E5" s="3">
         <v>6546546787</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="3">
+        <v>1235</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="22"/>
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -1324,18 +1334,21 @@
       <c r="E6" s="3">
         <v>6546546787</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="3">
+        <v>1237</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="23"/>
       <c r="B7" s="3">
         <v>4</v>
       </c>
@@ -1349,17 +1362,20 @@
         <v>5646876875</v>
       </c>
       <c r="F7" s="3">
+        <v>1236</v>
+      </c>
+      <c r="G7" s="3">
         <v>3</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1372,8 +1388,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="22"/>
       <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
@@ -1384,8 +1400,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="22"/>
       <c r="B11" s="3">
         <v>1</v>
       </c>
@@ -1396,8 +1412,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="22"/>
       <c r="B12" s="3">
         <v>2</v>
       </c>
@@ -1408,8 +1424,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="23"/>
       <c r="B13" s="3">
         <v>3</v>
       </c>
@@ -1420,8 +1436,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1431,8 +1447,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="22"/>
       <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
@@ -1441,7 +1457,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="3">
         <v>1</v>
       </c>
@@ -1450,7 +1466,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="3">
         <v>2</v>
       </c>
@@ -1459,7 +1475,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="3">
         <v>3</v>
       </c>
@@ -1468,7 +1484,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1494,7 +1510,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
@@ -1518,7 +1534,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="3">
         <v>1</v>
       </c>
@@ -1542,16 +1558,16 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
       <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="24" t="s">
         <v>53</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1562,7 +1578,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
+      <c r="A27" s="24"/>
       <c r="B27" s="2" t="s">
         <v>181</v>
       </c>
@@ -1571,7 +1587,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="3">
         <v>2</v>
       </c>
@@ -1580,7 +1596,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="17"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="3">
         <v>3</v>
       </c>
@@ -1589,7 +1605,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="21" t="s">
         <v>108</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1618,7 +1634,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="13"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="2" t="s">
         <v>25</v>
       </c>
@@ -1645,7 +1661,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="13"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="3">
         <v>1</v>
       </c>
@@ -1673,7 +1689,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="3">
         <v>2</v>
       </c>
@@ -1700,7 +1716,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="21" t="s">
         <v>119</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1723,7 +1739,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="13"/>
+      <c r="A38" s="22"/>
       <c r="B38" s="2" t="s">
         <v>25</v>
       </c>
@@ -1744,7 +1760,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="14"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="3">
         <v>1</v>
       </c>
@@ -1772,57 +1788,57 @@
       <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="15" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="13"/>
-      <c r="B42" s="21" t="s">
+      <c r="A42" s="22"/>
+      <c r="B42" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="C42" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D42" s="16" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="13"/>
-      <c r="B43" s="18">
+      <c r="A43" s="22"/>
+      <c r="B43" s="13">
         <v>1</v>
       </c>
-      <c r="C43" s="18">
+      <c r="C43" s="13">
         <v>1</v>
       </c>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="14" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="18">
+      <c r="A44" s="23"/>
+      <c r="B44" s="13">
         <v>2</v>
       </c>
-      <c r="C44" s="18">
+      <c r="C44" s="13">
         <v>1</v>
       </c>
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="14" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="21" t="s">
         <v>143</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -1839,7 +1855,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="13"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="2" t="s">
         <v>25</v>
       </c>
@@ -1854,7 +1870,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="13"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="3">
         <v>1</v>
       </c>
@@ -1869,7 +1885,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="14"/>
+      <c r="A49" s="23"/>
       <c r="B49" s="3">
         <v>2</v>
       </c>
@@ -1884,7 +1900,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="21" t="s">
         <v>152</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -1904,7 +1920,7 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="13"/>
+      <c r="A52" s="22"/>
       <c r="B52" s="2" t="s">
         <v>25</v>
       </c>
@@ -1922,7 +1938,7 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="14"/>
+      <c r="A53" s="23"/>
       <c r="B53" s="3">
         <v>1</v>
       </c>
@@ -1940,7 +1956,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="21" t="s">
         <v>183</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -1966,7 +1982,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="13"/>
+      <c r="A56" s="22"/>
       <c r="B56" s="2" t="s">
         <v>25</v>
       </c>
@@ -1990,7 +2006,7 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="14"/>
+      <c r="A57" s="23"/>
       <c r="B57" s="3">
         <v>1</v>
       </c>
@@ -2014,7 +2030,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="21" t="s">
         <v>178</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -2025,7 +2041,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="13"/>
+      <c r="A60" s="22"/>
       <c r="B60" s="2" t="s">
         <v>181</v>
       </c>
@@ -2034,7 +2050,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="14"/>
+      <c r="A61" s="23"/>
       <c r="B61" s="3">
         <v>1</v>
       </c>
@@ -2044,11 +2060,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A51:A53"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A32:A35"/>
     <mergeCell ref="A2:A7"/>
@@ -2056,6 +2067,11 @@
     <mergeCell ref="A22:A24"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A51:A53"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -2085,155 +2101,155 @@
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="27" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="27" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="27" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="14" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="14" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="14" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2261,173 +2277,168 @@
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="27" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="27" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="14">
         <v>30</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="27" t="s">
+      <c r="D9" s="14"/>
+      <c r="E9" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="20" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="F10" s="27"/>
+      <c r="F10" s="20"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="14" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="14" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2455,204 +2466,204 @@
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="27" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="27" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="27" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="14">
         <v>30</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="27" t="s">
+      <c r="D10" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="20" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="27" t="s">
+      <c r="D11" s="14"/>
+      <c r="E11" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="F11" s="27"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="27" t="s">
+      <c r="C12" s="14"/>
+      <c r="D12" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="F12" s="27"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="14" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="14" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2670,8 +2681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8788458-662F-3144-A12B-BEB3D3086BC2}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2680,123 +2691,123 @@
     <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="27" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="14" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="14" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="14" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2824,101 +2835,101 @@
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="14">
         <v>150</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="27" t="s">
+      <c r="D7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="14" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2946,133 +2957,133 @@
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="14">
         <v>150</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="27" t="s">
+      <c r="D7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="27" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="14" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3088,7 +3099,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A1FF0E-9F92-D34B-B956-2F4B42DFBB1D}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="75" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
@@ -3100,207 +3111,223 @@
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="14">
         <v>150</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="27" t="s">
+      <c r="D7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="14">
         <v>240</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="27" t="s">
+      <c r="D8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="14">
         <v>60</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="27" t="s">
+      <c r="D9" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="27"/>
-    </row>
-    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="F9" s="20"/>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="14">
+        <v>30</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10" s="20"/>
+    </row>
+    <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B11" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="27" t="s">
+      <c r="C11" s="14"/>
+      <c r="D11" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="27"/>
-    </row>
-    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
+      <c r="F11" s="20"/>
+    </row>
+    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B12" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C12" s="14">
         <v>30</v>
       </c>
-      <c r="D11" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="27" t="s">
+      <c r="D12" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F12" s="20" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+    <row r="13" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B13" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C13" s="14">
         <v>240</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D13" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E13" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="27"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="F13" s="20"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B15" s="17" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B16" s="14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B18" s="17" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B19" s="14" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3319,7 +3346,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3328,295 +3355,233 @@
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="14">
         <v>150</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="27" t="s">
+      <c r="D7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="14">
         <v>150</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="27" t="s">
+      <c r="D8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="14">
         <v>240</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="27" t="s">
+      <c r="D9" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="1:6" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="27" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="F10" s="27"/>
+      <c r="F10" s="20"/>
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="27" t="s">
+      <c r="C11" s="14"/>
+      <c r="D11" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="F11" s="27"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="14">
         <v>1000</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="27" t="s">
+      <c r="D12" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="27"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
+      <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D16" s="28"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D18" s="28"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="28"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="28"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F24" s="18"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F28" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3642,223 +3607,163 @@
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="27" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D11" s="28"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
+      <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3884,221 +3789,221 @@
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="27" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="14">
         <v>150</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="27" t="s">
+      <c r="D8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="14">
         <v>30</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="27" t="s">
+      <c r="D9" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="20" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="27" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="F10" s="27"/>
+      <c r="F10" s="20"/>
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="14">
         <v>240</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="F11" s="27"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19" t="s">
+      <c r="C12" s="14"/>
+      <c r="D12" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="F12" s="27"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="14">
         <v>1000</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="27" t="s">
+      <c r="D13" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="F13" s="27"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="14" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="14" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4126,191 +4031,191 @@
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="27" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="27" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="14">
         <v>30</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="27" t="s">
+      <c r="D9" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="20" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="27" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="F10" s="27"/>
+      <c r="F10" s="20"/>
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="27" t="s">
+      <c r="C11" s="14"/>
+      <c r="D11" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="F11" s="27"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="14" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="14" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="14" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4338,133 +4243,133 @@
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="27" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="14">
         <v>30</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="27" t="s">
+      <c r="D8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="14" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="14" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>